<commit_message>
DB e do-file updated!
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gills/Downloads/git-gills/2015-ciber-tri/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gills/Documents/academico/publicacoes/0 - Em confecção/RBPI - TRI e ciberespaço/cyber-irt/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="82">
   <si>
     <t>Limites e perspectivas da securitização: estudos de caso no contexto sulamericano contemporâneo</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>Frequency</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -803,6 +806,57 @@
       <right style="medium">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color auto="1"/>
@@ -900,7 +954,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1090,13 +1144,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1106,9 +1202,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1219,10 +1312,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1249,7 +1342,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1392,7 +1487,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1463,9 +1560,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="solid"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1544,11 +1641,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2100143888"/>
-        <c:axId val="2100147424"/>
+        <c:axId val="2126934416"/>
+        <c:axId val="2126930864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2100143888"/>
+        <c:axId val="2126934416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1688,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100147424"/>
+        <c:crossAx val="2126930864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1599,10 +1696,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100147424"/>
+        <c:axId val="2126930864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="160.0"/>
+          <c:max val="200.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1652,7 +1749,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100143888"/>
+        <c:crossAx val="2126934416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1779,10 +1876,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="105"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="5"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1798,13 +1895,43 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="19050">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:tint val="58000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:tint val="58000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:tint val="58000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3">
+                    <a:tint val="58000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1813,16 +1940,43 @@
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:tint val="86000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:tint val="86000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:tint val="86000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3">
+                    <a:tint val="86000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1831,13 +1985,43 @@
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="19050">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="86000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="86000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="86000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3">
+                    <a:shade val="86000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1846,13 +2030,43 @@
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="19050">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="58000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="58000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:shade val="58000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3">
+                    <a:shade val="58000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1872,9 +2086,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1893,14 +2110,13 @@
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
               <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:ln w="9525">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="35000"/>
                       <a:lumOff val="65000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:round/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
@@ -1933,21 +2149,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>IRt_PieGraph!$F$5:$F$8</c:f>
+              <c:f>IRt_PieGraph!$G$5:$G$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>0.555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>0.222222222222222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>0.111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.111111111111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1974,16 +2190,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0894868766404199"/>
-          <c:y val="0.769096675415573"/>
-          <c:w val="0.793248250218723"/>
-          <c:h val="0.19386628754739"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2000,8 +2207,8 @@
             <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -2022,7 +2229,12 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2046,82 +2258,35 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
   <cs:variation>
-    <a:lumMod val="60000"/>
+    <a:tint val="88500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
+    <a:tint val="55000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
+    <a:tint val="75000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
+    <a:tint val="98500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50000"/>
+    <a:tint val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
+    <a:tint val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
+    <a:tint val="80000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="23">
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -2629,18 +2794,18 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="254">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2648,8 +2813,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -2670,7 +2835,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2694,8 +2859,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2729,50 +2894,51 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr/>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="15875" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2784,30 +2950,33 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2824,20 +2993,18 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2847,7 +3014,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2856,14 +3023,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2872,17 +3038,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2891,17 +3057,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -2910,21 +3075,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2943,17 +3102,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2962,17 +3120,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2981,17 +3139,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3001,8 +3158,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3012,7 +3169,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -3020,7 +3177,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3029,10 +3186,21 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3040,17 +3208,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -3060,27 +3228,26 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3090,8 +3257,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3101,20 +3268,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3124,8 +3290,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3135,14 +3301,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3186,13 +3346,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>307733</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>196362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>234464</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>77178</xdr:rowOff>
@@ -3216,25 +3376,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>195383</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>113310</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>19539</xdr:rowOff>
+      <xdr:rowOff>15635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>634999</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>552926</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>19539</xdr:rowOff>
+      <xdr:rowOff>15635</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Chave Direita 3"/>
+        <xdr:cNvPr id="5" name="Chave Direita 4"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3057768" y="234462"/>
+          <a:off x="6092079" y="230558"/>
           <a:ext cx="439616" cy="2667000"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
@@ -3242,7 +3402,7 @@
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="FF0000"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
@@ -3273,33 +3433,33 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>113310</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>141920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>15635</xdr:rowOff>
+      <xdr:rowOff>14940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>552926</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>289436</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>15635</xdr:rowOff>
+      <xdr:rowOff>14940</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Chave Direita 4"/>
+        <xdr:cNvPr id="6" name="Chave Direita 5"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6092079" y="230558"/>
-          <a:ext cx="439616" cy="2667000"/>
+          <a:off x="2136567" y="231587"/>
+          <a:ext cx="147516" cy="2659529"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="FF0000"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
@@ -3598,7 +3758,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3762,10 +3922,10 @@
       </c>
     </row>
     <row r="10" spans="2:6" s="36" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="83"/>
       <c r="D10" s="4">
         <f>SUM(D3:D9)</f>
         <v>665</v>
@@ -3799,7 +3959,7 @@
   <sheetPr codeName="Plan2" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A44" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -4936,131 +5096,158 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F11"/>
+  <dimension ref="B1:G11"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="2" style="14" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="14" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="14"/>
+    <col min="3" max="3" width="19" style="13" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="18" style="14" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5" style="14" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="14" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" s="15" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+    <row r="1" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" s="15" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="71" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28">
+    <row r="3" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="66">
         <v>21</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="67" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="71">
+    <row r="4" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="84">
         <v>27</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="72" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="71"/>
-      <c r="C5" s="52" t="s">
+      <c r="G4" s="71" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="84"/>
+      <c r="C5" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="76">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="70">
+      <c r="G5" s="77">
+        <f>F5/F9</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="84">
         <v>34</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="64" t="s">
         <v>60</v>
       </c>
       <c r="E6" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="78">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="70"/>
+      <c r="G6" s="79">
+        <f>F6/F9</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="84"/>
       <c r="C7" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="78">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="49">
+      <c r="G7" s="79">
+        <f>F7/F9</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="65">
         <v>45</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="62">
+      <c r="F8" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="70">
+      <c r="G8" s="81">
+        <f>F8/F9</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="84">
         <v>47</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="67">
+      <c r="F9" s="74">
         <f>SUM(F5:F8)</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="70"/>
+      <c r="G9" s="75">
+        <f>SUM(G5:G8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="84"/>
       <c r="C10" s="64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="59">
+    <row r="11" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="68">
         <v>54</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="69" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>